<commit_message>
Corrected error on schematic & BOM
AD5040 was replaced with AD5060.
</commit_message>
<xml_diff>
--- a/Hardware/VoltageReferenceProgrammableRevDBOM.xlsx
+++ b/Hardware/VoltageReferenceProgrammableRevDBOM.xlsx
@@ -187,9 +187,6 @@
     <t>R7, R8, R9, R10, R11, R12, R13, R14</t>
   </si>
   <si>
-    <t>AD5040BRJZ</t>
-  </si>
-  <si>
     <t>SOT-23-8</t>
   </si>
   <si>
@@ -326,6 +323,9 @@
   </si>
   <si>
     <t>12k</t>
+  </si>
+  <si>
+    <t>AD5060BRJZ</t>
   </si>
 </sst>
 </file>
@@ -334,7 +334,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -414,7 +414,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -724,7 +724,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -924,7 +924,7 @@
         <v>3.8100000000000002E-2</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -1059,7 +1059,7 @@
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1140,7 +1140,7 @@
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -1167,16 +1167,16 @@
         <v>12.77</v>
       </c>
       <c r="D16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>49</v>
-      </c>
-      <c r="G16" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1191,16 +1191,16 @@
         <v>3.61</v>
       </c>
       <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>52</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>53</v>
-      </c>
-      <c r="G17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1215,19 +1215,19 @@
         <v>0.94399999999999995</v>
       </c>
       <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
         <v>55</v>
       </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>56</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>57</v>
-      </c>
-      <c r="H18" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1242,19 +1242,19 @@
         <v>0.57599999999999996</v>
       </c>
       <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
         <v>59</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>60</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>61</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>62</v>
-      </c>
-      <c r="H19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1269,19 +1269,19 @@
         <v>1.6850000000000001</v>
       </c>
       <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
         <v>64</v>
       </c>
-      <c r="E20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>65</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>66</v>
-      </c>
-      <c r="H20" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1296,19 +1296,19 @@
         <v>0.64400000000000002</v>
       </c>
       <c r="D21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
         <v>68</v>
       </c>
-      <c r="E21" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>69</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>70</v>
-      </c>
-      <c r="H21" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1323,19 +1323,19 @@
         <v>0.37440000000000001</v>
       </c>
       <c r="D22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" t="s">
         <v>72</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>73</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>75</v>
-      </c>
-      <c r="H22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1350,16 +1350,16 @@
         <v>7.31</v>
       </c>
       <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" t="s">
         <v>77</v>
       </c>
-      <c r="E23" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>78</v>
-      </c>
-      <c r="G23" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1374,19 +1374,19 @@
         <v>0.36799999999999999</v>
       </c>
       <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
         <v>80</v>
       </c>
-      <c r="E24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>81</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>82</v>
-      </c>
-      <c r="H24" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1401,16 +1401,16 @@
         <v>2.95</v>
       </c>
       <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
         <v>84</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>85</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>86</v>
-      </c>
-      <c r="G25" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
         <v>5.7333333333333334</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1436,7 +1436,7 @@
         <v>43.891433333333339</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM to note potential part subst
to make assembly easier for some folks.
</commit_message>
<xml_diff>
--- a/Hardware/VoltageReferenceProgrammableRevDBOM.xlsx
+++ b/Hardware/VoltageReferenceProgrammableRevDBOM.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="VoltageReferenceProgrammableRevDBOM" localSheetId="0">Sheet1!$A$1:$M$25</definedName>
+    <definedName name="VoltageReferenceProgrammableRevDBOM" localSheetId="0">Sheet1!$A$2:$M$26</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
   <si>
     <t>Qty</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>AD5060BRJZ</t>
+  </si>
+  <si>
+    <t>NOTE: Altitude on the SparkFun forum points out that the pads for the 0805 parts below are small for hand soldering and that substituting 0603 parts where possible actually makes assembly easier.  If this works for you, there is no functional downside to using the 0603 parts. Thx. - CS</t>
   </si>
 </sst>
 </file>
@@ -721,11 +724,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -742,96 +743,74 @@
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1.41E-2</v>
-      </c>
-      <c r="C2" s="3">
-        <f>A2*B2</f>
-        <v>8.4599999999999995E-2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>805</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6">
-        <v>1.2200000000000001E-2</v>
+        <v>1.41E-2</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C26" si="0">A3*B3</f>
-        <v>1.2200000000000001E-2</v>
+        <f>A3*B3</f>
+        <v>8.4599999999999995E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>805</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -839,14 +818,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="6">
-        <v>1.6199999999999999E-2</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6199999999999999E-2</v>
+        <f t="shared" ref="C4:C27" si="0">A4*B4</f>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -855,7 +834,7 @@
         <v>805</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -863,80 +842,80 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="6">
-        <v>4.99E-2</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>0.1996</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>805</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.83699999999999997</v>
+        <v>4.99E-2</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>4.1849999999999996</v>
+        <v>0.1996</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>805</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>3.8100000000000002E-2</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>3.8100000000000002E-2</v>
+        <v>4.1849999999999996</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7">
-        <v>805</v>
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -944,26 +923,26 @@
         <v>1</v>
       </c>
       <c r="B8" s="6">
-        <v>0.4</v>
+        <v>3.8100000000000002E-2</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>3.8100000000000002E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>805</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -971,80 +950,80 @@
         <v>1</v>
       </c>
       <c r="B9" s="6">
-        <v>3.85E-2</v>
+        <v>0.4</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>3.85E-2</v>
+        <v>0.4</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9">
-        <v>805</v>
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="6">
-        <v>0.104</v>
+        <v>3.85E-2</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>0.20799999999999999</v>
+        <v>3.85E-2</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F10">
         <v>805</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="6">
-        <v>7.1000000000000004E-3</v>
+        <v>0.104</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="0"/>
-        <v>7.1000000000000004E-3</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F11">
         <v>805</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1052,14 +1031,14 @@
         <v>1</v>
       </c>
       <c r="B12" s="6">
-        <v>1.2200000000000001E-2</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>1.2200000000000001E-2</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1068,7 +1047,7 @@
         <v>805</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" t="s">
         <v>17</v>
@@ -1079,14 +1058,14 @@
         <v>1</v>
       </c>
       <c r="B13" s="6">
-        <v>8.3999999999999995E-3</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="0"/>
-        <v>8.3999999999999995E-3</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -1095,7 +1074,7 @@
         <v>805</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
@@ -1106,77 +1085,80 @@
         <v>1</v>
       </c>
       <c r="B14" s="6">
-        <v>1.66</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="0"/>
-        <v>1.66</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" t="s">
-        <v>44</v>
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>805</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B15" s="6">
-        <v>7.1000000000000004E-3</v>
+        <v>1.66</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="0"/>
-        <v>5.6800000000000003E-2</v>
+        <v>1.66</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15">
-        <v>805</v>
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H15" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B16" s="6">
-        <v>12.77</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="0"/>
-        <v>12.77</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" t="s">
-        <v>48</v>
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>805</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1184,23 +1166,23 @@
         <v>1</v>
       </c>
       <c r="B17" s="6">
-        <v>3.61</v>
+        <v>12.77</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="0"/>
-        <v>3.61</v>
+        <v>12.77</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1208,26 +1190,23 @@
         <v>1</v>
       </c>
       <c r="B18" s="6">
-        <v>0.94399999999999995</v>
+        <v>3.61</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="0"/>
-        <v>0.94399999999999995</v>
+        <v>3.61</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1235,26 +1214,26 @@
         <v>1</v>
       </c>
       <c r="B19" s="6">
-        <v>0.57599999999999996</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1262,26 +1241,26 @@
         <v>1</v>
       </c>
       <c r="B20" s="6">
-        <v>1.6850000000000001</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="0"/>
-        <v>1.6850000000000001</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1289,77 +1268,80 @@
         <v>1</v>
       </c>
       <c r="B21" s="6">
-        <v>0.64400000000000002</v>
+        <v>1.6850000000000001</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="0"/>
-        <v>0.64400000000000002</v>
+        <v>1.6850000000000001</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="6">
-        <v>0.18720000000000001</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="0"/>
-        <v>0.37440000000000001</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H22" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="6">
-        <v>7.31</v>
+        <v>0.18720000000000001</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="0"/>
-        <v>7.31</v>
+        <v>0.37440000000000001</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1367,26 +1349,23 @@
         <v>1</v>
       </c>
       <c r="B24" s="6">
-        <v>0.36799999999999999</v>
+        <v>7.31</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="0"/>
-        <v>0.36799999999999999</v>
+        <v>7.31</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G24" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1394,23 +1373,26 @@
         <v>1</v>
       </c>
       <c r="B25" s="6">
-        <v>2.95</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="0"/>
-        <v>2.95</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="H25" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1418,24 +1400,48 @@
         <v>1</v>
       </c>
       <c r="B26" s="6">
+        <v>2.95</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>2.95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6">
         <f>17.2/3</f>
         <v>5.7333333333333334</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C27" s="3">
         <f t="shared" si="0"/>
         <v>5.7333333333333334</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="4">
-        <f>SUM(C2:C27)</f>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="4">
+        <f>SUM(C3:C28)</f>
         <v>43.891433333333339</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>